<commit_message>
update: added salad ingredients
</commit_message>
<xml_diff>
--- a/Salad/Salad_planner_database.xlsx
+++ b/Salad/Salad_planner_database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yolandatiao/Documents/YoloCookBlob/Salad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D32C27B-67D2-C44B-9FA0-208BE70523FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2932029-2172-354E-B4F2-069FE6161085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21820" yWindow="-18920" windowWidth="28040" windowHeight="15700" xr2:uid="{01A3236E-6E79-A74A-AA94-09FBDF0EA52A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15700" xr2:uid="{01A3236E-6E79-A74A-AA94-09FBDF0EA52A}"/>
   </bookViews>
   <sheets>
     <sheet name="database" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="196">
   <si>
     <t>Name</t>
   </si>
@@ -77,15 +77,6 @@
     <t>Cucumbers</t>
   </si>
   <si>
-    <t>Green peas</t>
-  </si>
-  <si>
-    <t>Chick peas</t>
-  </si>
-  <si>
-    <t>Button mushrooms</t>
-  </si>
-  <si>
     <t>Fruits</t>
   </si>
   <si>
@@ -122,9 +113,6 @@
     <t>ProteinFat</t>
   </si>
   <si>
-    <t>Hard boiled egg</t>
-  </si>
-  <si>
     <t>Avocado</t>
   </si>
   <si>
@@ -134,15 +122,6 @@
     <t>Edamame</t>
   </si>
   <si>
-    <t>Roasted chicken breast</t>
-  </si>
-  <si>
-    <t>Gilled salmon</t>
-  </si>
-  <si>
-    <t>Grilled shrimp</t>
-  </si>
-  <si>
     <t>Ham</t>
   </si>
   <si>
@@ -188,24 +167,9 @@
     <t>Raisins</t>
   </si>
   <si>
-    <t>Dried cranberries</t>
-  </si>
-  <si>
-    <t>Dried figs</t>
-  </si>
-  <si>
-    <t>Dried plums</t>
-  </si>
-  <si>
     <t>Arugula</t>
   </si>
   <si>
-    <t>Basil / Thai basil</t>
-  </si>
-  <si>
-    <t>Mint / lemon balm</t>
-  </si>
-  <si>
     <t>Dill</t>
   </si>
   <si>
@@ -221,24 +185,15 @@
     <t>HerbFlavor</t>
   </si>
   <si>
-    <t>Roasted garlic</t>
-  </si>
-  <si>
     <t>Jalapeno</t>
   </si>
   <si>
     <t>Pickles</t>
   </si>
   <si>
-    <t>Non fat greek yogurt &amp; olive oil &amp; chive dressing</t>
-  </si>
-  <si>
     <t>Sriracha</t>
   </si>
   <si>
-    <t>Lemon juice</t>
-  </si>
-  <si>
     <t>LightDressingSeasoning</t>
   </si>
   <si>
@@ -266,12 +221,6 @@
     <t>Green</t>
   </si>
   <si>
-    <t>Broccoli / cauliflower (air fried / roasted)</t>
-  </si>
-  <si>
-    <t>Brussel sprouts (air fried / roasted)</t>
-  </si>
-  <si>
     <t>Yellow</t>
   </si>
   <si>
@@ -287,21 +236,9 @@
     <t>Beets (boiled)</t>
   </si>
   <si>
-    <t>Low fat 2% cottage cheese</t>
-  </si>
-  <si>
     <t>Orange</t>
   </si>
   <si>
-    <t>Hard cheese (1 oz cube or shredded)</t>
-  </si>
-  <si>
-    <t>Grilled white fish (Tilapia)</t>
-  </si>
-  <si>
-    <t>Bacon crumbles</t>
-  </si>
-  <si>
     <t>Butternut squash (air fried / roasted)</t>
   </si>
   <si>
@@ -311,9 +248,6 @@
     <t>Salt &amp; Pepper</t>
   </si>
   <si>
-    <t>Balsamic vinegar</t>
-  </si>
-  <si>
     <t>RUV_1</t>
   </si>
   <si>
@@ -549,6 +483,147 @@
   </si>
   <si>
     <t>Protein (g)</t>
+  </si>
+  <si>
+    <t>HBF_11</t>
+  </si>
+  <si>
+    <t>Sauerkraut</t>
+  </si>
+  <si>
+    <t>HBF_12</t>
+  </si>
+  <si>
+    <t>Artichoke Hearts</t>
+  </si>
+  <si>
+    <t>HBF_13</t>
+  </si>
+  <si>
+    <t>Kimchi</t>
+  </si>
+  <si>
+    <t>HBF_14</t>
+  </si>
+  <si>
+    <t>Black Pearls Chopped Ripe Olives</t>
+  </si>
+  <si>
+    <t>LDS_5</t>
+  </si>
+  <si>
+    <t>Cedar's Original Hummus</t>
+  </si>
+  <si>
+    <t>CRB_17</t>
+  </si>
+  <si>
+    <t>Kamut</t>
+  </si>
+  <si>
+    <t>PRT_15</t>
+  </si>
+  <si>
+    <t>PRT_16</t>
+  </si>
+  <si>
+    <t>Romesco Dip</t>
+  </si>
+  <si>
+    <t>HDS_2</t>
+  </si>
+  <si>
+    <t>Ranch Dressing</t>
+  </si>
+  <si>
+    <t>Balsamic Vinegar</t>
+  </si>
+  <si>
+    <t>Lemon Juice</t>
+  </si>
+  <si>
+    <t>Roasted Garlic</t>
+  </si>
+  <si>
+    <t>Mint / Lemon Balm</t>
+  </si>
+  <si>
+    <t>Basil / Thai Basil</t>
+  </si>
+  <si>
+    <t>Dried Plums</t>
+  </si>
+  <si>
+    <t>Dried Figs</t>
+  </si>
+  <si>
+    <t>Dried Cranberries</t>
+  </si>
+  <si>
+    <t>Bacon Crumbles</t>
+  </si>
+  <si>
+    <t>Grilled Shrimp</t>
+  </si>
+  <si>
+    <t>Grilled White Fish (Tilapia)</t>
+  </si>
+  <si>
+    <t>Gilled Salmon</t>
+  </si>
+  <si>
+    <t>Roasted Chicken Breast</t>
+  </si>
+  <si>
+    <t>Chick Peas</t>
+  </si>
+  <si>
+    <t>Roasted Chopped Chicken with Skin</t>
+  </si>
+  <si>
+    <t>Roasted Chopped Turkey</t>
+  </si>
+  <si>
+    <t>Hard Cheese (1 oz cube or shredded)</t>
+  </si>
+  <si>
+    <t>Low Fat 2% Cottage Cheese</t>
+  </si>
+  <si>
+    <t>Hard  Boiled Egg</t>
+  </si>
+  <si>
+    <t>Broccoli / Cauliflower (air fried / roasted)</t>
+  </si>
+  <si>
+    <t>Brussel Sprouts (air fried / roasted)</t>
+  </si>
+  <si>
+    <t>Button Mushrooms</t>
+  </si>
+  <si>
+    <t>Green Peas</t>
+  </si>
+  <si>
+    <t>Thousand Island Dressing</t>
+  </si>
+  <si>
+    <t>Maple Basamic Vinaigrette</t>
+  </si>
+  <si>
+    <t>HDS_3</t>
+  </si>
+  <si>
+    <t>HDS_4</t>
+  </si>
+  <si>
+    <t>Vinaigrette</t>
+  </si>
+  <si>
+    <t>HDS_5</t>
+  </si>
+  <si>
+    <t>Cranberry Sauce</t>
   </si>
 </sst>
 </file>
@@ -998,11 +1073,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17DD8FDC-0274-0A43-8E33-FB5447076196}">
-  <dimension ref="A1:O73"/>
+  <dimension ref="A1:O86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K1" sqref="K1"/>
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1034,40 +1109,40 @@
         <v>0</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>165</v>
+        <v>143</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>166</v>
+        <v>144</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>167</v>
+        <v>145</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>168</v>
+        <v>146</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>169</v>
+        <v>147</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>170</v>
+        <v>148</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="N1" s="13" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="O1" s="13" t="s">
-        <v>164</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -1075,13 +1150,13 @@
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E2" s="1">
         <v>227</v>
@@ -1121,13 +1196,13 @@
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>112</v>
+        <v>90</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E3" s="1">
         <v>58</v>
@@ -1154,11 +1229,11 @@
         <v>0.8</v>
       </c>
       <c r="N3" s="14">
-        <f t="shared" ref="N3:N66" si="0">F3*15/240</f>
+        <f t="shared" ref="N3:N69" si="0">F3*15/240</f>
         <v>0.5</v>
       </c>
       <c r="O3" s="14">
-        <f t="shared" ref="O3:O66" si="1">F3/E3</f>
+        <f t="shared" ref="O3:O69" si="1">F3/E3</f>
         <v>0.13793103448275862</v>
       </c>
     </row>
@@ -1167,13 +1242,13 @@
         <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E4" s="1">
         <v>89</v>
@@ -1213,13 +1288,13 @@
         <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E5" s="1">
         <v>130</v>
@@ -1259,13 +1334,13 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E6" s="1">
         <v>180</v>
@@ -1305,13 +1380,13 @@
         <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>116</v>
+        <v>94</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E7" s="1">
         <v>20</v>
@@ -1351,13 +1426,13 @@
         <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>117</v>
+        <v>95</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E8" s="1">
         <v>37.5</v>
@@ -1397,13 +1472,13 @@
         <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E9" s="1">
         <v>25</v>
@@ -1440,16 +1515,16 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E10" s="1">
         <v>148</v>
@@ -1486,16 +1561,16 @@
     </row>
     <row r="11" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E11" s="1">
         <v>120</v>
@@ -1532,16 +1607,16 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E12" s="1">
         <v>129</v>
@@ -1581,16 +1656,16 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>13</v>
+        <v>188</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E13" s="1">
         <v>160</v>
@@ -1627,16 +1702,16 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>15</v>
+        <v>187</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E14" s="1">
         <v>78.8</v>
@@ -1673,16 +1748,16 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E15" s="1">
         <v>117</v>
@@ -1719,16 +1794,16 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E16" s="1">
         <v>172</v>
@@ -1765,16 +1840,16 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>76</v>
+        <v>185</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E17" s="1">
         <v>170</v>
@@ -1811,16 +1886,16 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>77</v>
+        <v>186</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E18" s="1">
         <v>162</v>
@@ -1857,16 +1932,16 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E19" s="1">
         <v>145</v>
@@ -1903,16 +1978,16 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E20" s="1">
         <v>176.5</v>
@@ -1952,16 +2027,16 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="D21" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E21" s="1">
         <v>165</v>
@@ -2001,16 +2076,16 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E22" s="1">
         <v>169</v>
@@ -2047,16 +2122,16 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E23" s="1">
         <v>376</v>
@@ -2096,16 +2171,16 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E24" s="1">
         <v>221</v>
@@ -2142,16 +2217,16 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E25" s="1">
         <v>144</v>
@@ -2188,16 +2263,16 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E26" s="1">
         <v>151</v>
@@ -2237,16 +2312,16 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E27" s="1">
         <v>153</v>
@@ -2286,16 +2361,16 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E28" s="1">
         <v>194</v>
@@ -2335,16 +2410,16 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>119</v>
+        <v>97</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>28</v>
+        <v>184</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="E29" s="1">
         <v>135</v>
@@ -2384,16 +2459,16 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="E30" s="1">
         <v>150</v>
@@ -2433,16 +2508,16 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>83</v>
+        <v>183</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="E31" s="1">
         <v>226</v>
@@ -2479,16 +2554,16 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>85</v>
+        <v>182</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="E32" s="1">
         <v>240</v>
@@ -2528,16 +2603,16 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="E33" s="1">
         <v>227</v>
@@ -2574,16 +2649,16 @@
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="D34" s="1" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="E34" s="1">
         <v>107</v>
@@ -2620,74 +2695,74 @@
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>14</v>
+        <v>181</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="E35" s="1">
-        <v>164</v>
+        <v>140</v>
       </c>
       <c r="F35" s="2">
-        <v>269</v>
+        <v>238</v>
       </c>
       <c r="G35" s="3">
-        <v>4.2</v>
+        <v>7</v>
       </c>
       <c r="H35" s="3">
-        <v>0.4</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="I35" s="4">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="J35" s="4">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="K35" s="4">
-        <v>7.9</v>
+        <v>0</v>
       </c>
       <c r="L35" s="5">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="N35" s="14">
         <f t="shared" si="0"/>
-        <v>16.8125</v>
+        <v>14.875</v>
       </c>
       <c r="O35" s="14">
         <f t="shared" si="1"/>
-        <v>1.6402439024390243</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>32</v>
+        <v>180</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="E36" s="1">
-        <v>187</v>
+        <v>135</v>
       </c>
       <c r="F36" s="2">
-        <v>100</v>
+        <v>320</v>
       </c>
       <c r="G36" s="3">
-        <v>1.67</v>
+        <v>18.2</v>
       </c>
       <c r="H36" s="3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I36" s="4">
         <v>0</v>
@@ -2699,400 +2774,400 @@
         <v>0</v>
       </c>
       <c r="L36" s="5">
-        <v>21.7</v>
-      </c>
-      <c r="M36" s="2">
-        <v>193</v>
+        <v>36.6</v>
       </c>
       <c r="N36" s="14">
         <f t="shared" si="0"/>
-        <v>6.25</v>
+        <v>20</v>
       </c>
       <c r="O36" s="14">
         <f t="shared" si="1"/>
-        <v>0.53475935828877008</v>
+        <v>2.3703703703703702</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>33</v>
+        <v>179</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="E37" s="1">
-        <v>136</v>
+        <v>164</v>
       </c>
       <c r="F37" s="2">
-        <v>233</v>
+        <v>269</v>
       </c>
       <c r="G37" s="3">
-        <v>10.3</v>
+        <v>4.2</v>
       </c>
       <c r="H37" s="3">
-        <v>1.8</v>
+        <v>0.4</v>
       </c>
       <c r="I37" s="4">
-        <v>0.7</v>
+        <v>45</v>
       </c>
       <c r="J37" s="4">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="K37" s="4">
-        <v>0.2</v>
+        <v>7.9</v>
       </c>
       <c r="L37" s="5">
-        <v>32.6</v>
+        <v>15</v>
       </c>
       <c r="N37" s="14">
         <f t="shared" si="0"/>
-        <v>14.5625</v>
+        <v>16.8125</v>
       </c>
       <c r="O37" s="14">
         <f t="shared" si="1"/>
-        <v>1.713235294117647</v>
+        <v>1.6402439024390243</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>86</v>
+        <v>178</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="E38" s="1">
-        <v>136</v>
+        <v>187</v>
       </c>
       <c r="F38" s="2">
-        <v>148</v>
+        <v>100</v>
       </c>
       <c r="G38" s="3">
-        <v>1.6</v>
+        <v>1.67</v>
       </c>
       <c r="H38" s="3">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="I38" s="4">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="J38" s="4">
         <v>0</v>
       </c>
       <c r="K38" s="4">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="L38" s="5">
-        <v>30.7</v>
+        <v>21.7</v>
+      </c>
+      <c r="M38" s="2">
+        <v>193</v>
       </c>
       <c r="N38" s="14">
         <f t="shared" si="0"/>
-        <v>9.25</v>
+        <v>6.25</v>
       </c>
       <c r="O38" s="14">
         <f t="shared" si="1"/>
-        <v>1.088235294117647</v>
+        <v>0.53475935828877008</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>34</v>
+        <v>177</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="E39" s="1">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="F39" s="2">
-        <v>171</v>
+        <v>233</v>
       </c>
       <c r="G39" s="3">
-        <v>2.4</v>
+        <v>10.3</v>
       </c>
       <c r="H39" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="I39" s="4">
         <v>0.7</v>
       </c>
-      <c r="I39" s="4">
-        <v>2.2000000000000002</v>
-      </c>
       <c r="J39" s="4">
         <v>0</v>
       </c>
       <c r="K39" s="4">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="L39" s="5">
-        <v>32</v>
+        <v>32.6</v>
       </c>
       <c r="N39" s="14">
         <f t="shared" si="0"/>
-        <v>10.6875</v>
+        <v>14.5625</v>
       </c>
       <c r="O39" s="14">
         <f t="shared" si="1"/>
-        <v>1.1875</v>
+        <v>1.713235294117647</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>130</v>
+        <v>108</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>87</v>
+        <v>176</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="E40" s="1">
-        <v>112</v>
+        <v>136</v>
       </c>
       <c r="F40" s="2">
-        <v>480</v>
+        <v>148</v>
       </c>
       <c r="G40" s="3">
-        <v>32</v>
+        <v>1.6</v>
       </c>
       <c r="H40" s="3">
-        <v>16</v>
+        <v>0.3</v>
       </c>
       <c r="I40" s="4">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="J40" s="4">
         <v>0</v>
       </c>
       <c r="K40" s="4">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="L40" s="5">
-        <v>32</v>
+        <v>30.7</v>
       </c>
       <c r="N40" s="14">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>9.25</v>
       </c>
       <c r="O40" s="14">
         <f t="shared" si="1"/>
-        <v>4.2857142857142856</v>
+        <v>1.088235294117647</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>35</v>
+        <v>175</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="E41" s="1">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="F41" s="2">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="G41" s="3">
-        <v>6.8</v>
+        <v>2.4</v>
       </c>
       <c r="H41" s="3">
-        <v>1.3</v>
+        <v>0.7</v>
       </c>
       <c r="I41" s="4">
-        <v>1.4</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="J41" s="4">
         <v>0</v>
       </c>
       <c r="K41" s="4">
-        <v>1.4</v>
+        <v>0</v>
       </c>
       <c r="L41" s="5">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="N41" s="14">
         <f t="shared" si="0"/>
-        <v>11.625</v>
+        <v>10.6875</v>
       </c>
       <c r="O41" s="14">
         <f t="shared" si="1"/>
-        <v>1.3880597014925373</v>
+        <v>1.1875</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>36</v>
+        <v>174</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="E42" s="1">
-        <v>142</v>
+        <v>112</v>
       </c>
       <c r="F42" s="2">
-        <v>858</v>
+        <v>480</v>
       </c>
       <c r="G42" s="3">
-        <v>76</v>
+        <v>32</v>
       </c>
       <c r="H42" s="3">
-        <v>16.5</v>
+        <v>16</v>
       </c>
       <c r="I42" s="4">
-        <v>29.8</v>
+        <v>0</v>
       </c>
       <c r="J42" s="4">
-        <v>10.8</v>
+        <v>0</v>
       </c>
       <c r="K42" s="4">
-        <v>6.4</v>
+        <v>0</v>
       </c>
       <c r="L42" s="5">
-        <v>27.8</v>
+        <v>32</v>
       </c>
       <c r="N42" s="14">
         <f t="shared" si="0"/>
-        <v>53.625</v>
+        <v>30</v>
       </c>
       <c r="O42" s="14">
         <f t="shared" si="1"/>
-        <v>6.042253521126761</v>
+        <v>4.2857142857142856</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>133</v>
+        <v>161</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="E43" s="1">
-        <v>100</v>
+        <v>134</v>
       </c>
       <c r="F43" s="2">
-        <v>150</v>
+        <v>186</v>
       </c>
       <c r="G43" s="3">
-        <v>7.5</v>
+        <v>6.8</v>
       </c>
       <c r="H43" s="3">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="I43" s="4">
-        <v>19.5</v>
+        <v>1.4</v>
       </c>
       <c r="J43" s="4">
-        <v>3.2</v>
+        <v>0</v>
       </c>
       <c r="K43" s="4">
-        <v>6</v>
+        <v>1.4</v>
       </c>
       <c r="L43" s="5">
-        <v>1.9</v>
+        <v>30</v>
       </c>
       <c r="N43" s="14">
         <f t="shared" si="0"/>
-        <v>9.375</v>
+        <v>11.625</v>
       </c>
       <c r="O43" s="14">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>1.3880597014925373</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>134</v>
+        <v>162</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E44" s="1">
-        <v>209</v>
+        <v>142</v>
       </c>
       <c r="F44" s="2">
-        <v>108</v>
+        <v>858</v>
       </c>
       <c r="G44" s="3">
-        <v>6.3</v>
+        <v>76</v>
       </c>
       <c r="H44" s="3">
-        <v>0.9</v>
+        <v>16.5</v>
       </c>
       <c r="I44" s="4">
-        <v>14</v>
+        <v>29.8</v>
       </c>
       <c r="J44" s="4">
-        <v>1.2</v>
+        <v>10.8</v>
       </c>
       <c r="K44" s="4">
-        <v>5.6</v>
+        <v>6.4</v>
       </c>
       <c r="L44" s="5">
-        <v>2.1</v>
+        <v>27.8</v>
       </c>
       <c r="N44" s="14">
         <f t="shared" si="0"/>
-        <v>6.75</v>
+        <v>53.625</v>
       </c>
       <c r="O44" s="14">
         <f t="shared" si="1"/>
-        <v>0.51674641148325362</v>
+        <v>6.042253521126761</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>135</v>
+        <v>111</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="E45" s="1">
         <v>100</v>
@@ -3101,16 +3176,16 @@
         <v>150</v>
       </c>
       <c r="G45" s="3">
-        <v>7.4</v>
+        <v>7.5</v>
       </c>
       <c r="H45" s="3">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="I45" s="4">
-        <v>19</v>
+        <v>19.5</v>
       </c>
       <c r="J45" s="4">
-        <v>3.1</v>
+        <v>3.2</v>
       </c>
       <c r="K45" s="4">
         <v>6</v>
@@ -3129,764 +3204,764 @@
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="E46" s="1">
-        <v>157</v>
+        <v>209</v>
       </c>
       <c r="F46" s="2">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G46" s="3">
-        <v>0.5</v>
+        <v>6.3</v>
       </c>
       <c r="H46" s="3">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="I46" s="4">
-        <v>26.8</v>
+        <v>14</v>
       </c>
       <c r="J46" s="4">
-        <v>5.7</v>
+        <v>1.2</v>
       </c>
       <c r="K46" s="4">
-        <v>7.6</v>
+        <v>5.6</v>
       </c>
       <c r="L46" s="5">
-        <v>2</v>
+        <v>2.1</v>
       </c>
       <c r="N46" s="14">
         <f t="shared" si="0"/>
-        <v>6.9375</v>
+        <v>6.75</v>
       </c>
       <c r="O46" s="14">
-        <f>F46/E46</f>
-        <v>0.70700636942675155</v>
+        <f t="shared" si="1"/>
+        <v>0.51674641148325362</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>137</v>
+        <v>113</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>88</v>
+        <v>36</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="E47" s="1">
-        <v>205</v>
+        <v>100</v>
       </c>
       <c r="F47" s="2">
-        <v>82</v>
+        <v>150</v>
       </c>
       <c r="G47" s="3">
-        <v>0.2</v>
+        <v>7.4</v>
       </c>
       <c r="H47" s="3">
-        <v>0</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="I47" s="4">
-        <v>21.5</v>
+        <v>19</v>
       </c>
       <c r="J47" s="4">
-        <v>6.6</v>
+        <v>3.1</v>
       </c>
       <c r="K47" s="4">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="L47" s="5">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="N47" s="14">
         <f t="shared" si="0"/>
-        <v>5.125</v>
+        <v>9.375</v>
       </c>
       <c r="O47" s="14">
         <f t="shared" si="1"/>
-        <v>0.4</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="D48" s="1" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="E48" s="1">
-        <v>112.5</v>
+        <v>157</v>
       </c>
       <c r="F48" s="2">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="G48" s="3">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="H48" s="3">
         <v>0</v>
       </c>
       <c r="I48" s="4">
-        <v>24</v>
+        <v>26.8</v>
       </c>
       <c r="J48" s="4">
+        <v>5.7</v>
+      </c>
+      <c r="K48" s="4">
+        <v>7.6</v>
+      </c>
+      <c r="L48" s="5">
         <v>2</v>
       </c>
-      <c r="K48" s="4">
-        <v>1.8</v>
-      </c>
-      <c r="L48" s="5">
-        <v>2.8</v>
-      </c>
       <c r="N48" s="14">
-        <f>F48*15/240</f>
-        <v>6.8125</v>
+        <f t="shared" si="0"/>
+        <v>6.9375</v>
       </c>
       <c r="O48" s="14">
-        <f t="shared" si="1"/>
-        <v>0.96888888888888891</v>
+        <f>F48/E48</f>
+        <v>0.70700636942675155</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>139</v>
+        <v>115</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="E49" s="1">
-        <v>150</v>
+        <v>205</v>
       </c>
       <c r="F49" s="2">
-        <v>129</v>
+        <v>82</v>
       </c>
       <c r="G49" s="3">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="H49" s="3">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="I49" s="4">
-        <v>28</v>
+        <v>21.5</v>
       </c>
       <c r="J49" s="4">
-        <v>3</v>
+        <v>6.6</v>
       </c>
       <c r="K49" s="4">
-        <v>9.4</v>
+        <v>1</v>
       </c>
       <c r="L49" s="5">
-        <v>4.9000000000000004</v>
+        <v>1.8</v>
       </c>
       <c r="N49" s="14">
         <f t="shared" si="0"/>
-        <v>8.0625</v>
+        <v>5.125</v>
       </c>
       <c r="O49" s="14">
         <f t="shared" si="1"/>
-        <v>0.86</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>140</v>
+        <v>116</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="E50" s="1">
-        <v>186</v>
+        <v>112.5</v>
       </c>
       <c r="F50" s="2">
-        <v>222</v>
+        <v>109</v>
       </c>
       <c r="G50" s="3">
-        <v>3.6</v>
+        <v>0.2</v>
       </c>
       <c r="H50" s="3">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="I50" s="4">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="J50" s="4">
-        <v>5.2</v>
+        <v>2</v>
       </c>
       <c r="K50" s="4">
-        <v>1.6</v>
+        <v>1.8</v>
       </c>
       <c r="L50" s="5">
-        <v>8.1999999999999993</v>
+        <v>2.8</v>
       </c>
       <c r="N50" s="14">
-        <f t="shared" si="0"/>
-        <v>13.875</v>
+        <f>F50*15/240</f>
+        <v>6.8125</v>
       </c>
       <c r="O50" s="14">
         <f t="shared" si="1"/>
-        <v>1.1935483870967742</v>
+        <v>0.96888888888888891</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>141</v>
+        <v>117</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E51" s="1">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="F51" s="2">
-        <v>198</v>
+        <v>129</v>
       </c>
       <c r="G51" s="3">
-        <v>0.7</v>
+        <v>2</v>
       </c>
       <c r="H51" s="3">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="I51" s="4">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="J51" s="4">
-        <v>6.2</v>
+        <v>3</v>
       </c>
       <c r="K51" s="4">
-        <v>0.4</v>
+        <v>9.4</v>
       </c>
       <c r="L51" s="5">
-        <v>3.6</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="N51" s="14">
         <f t="shared" si="0"/>
-        <v>12.375</v>
+        <v>8.0625</v>
       </c>
       <c r="O51" s="14">
         <f t="shared" si="1"/>
-        <v>1.2298136645962734</v>
+        <v>0.86</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>142</v>
+        <v>118</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="E52" s="1">
-        <v>164</v>
+        <v>186</v>
       </c>
       <c r="F52" s="2">
-        <v>166</v>
+        <v>222</v>
       </c>
       <c r="G52" s="3">
-        <v>0.6</v>
+        <v>3.6</v>
       </c>
       <c r="H52" s="3">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="I52" s="4">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="J52" s="4">
-        <v>3</v>
+        <v>5.2</v>
       </c>
       <c r="K52" s="4">
-        <v>1.2</v>
+        <v>1.6</v>
       </c>
       <c r="L52" s="5">
-        <v>6.5</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="N52" s="14">
         <f t="shared" si="0"/>
-        <v>10.375</v>
+        <v>13.875</v>
       </c>
       <c r="O52" s="14">
         <f t="shared" si="1"/>
-        <v>1.0121951219512195</v>
+        <v>1.1935483870967742</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>143</v>
+        <v>119</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E53" s="1">
-        <v>195</v>
+        <v>161</v>
       </c>
       <c r="F53" s="2">
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="G53" s="3">
-        <v>1.5</v>
+        <v>0.7</v>
       </c>
       <c r="H53" s="3">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="I53" s="4">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="J53" s="4">
-        <v>2</v>
+        <v>6.2</v>
       </c>
       <c r="K53" s="4">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="L53" s="5">
-        <v>3</v>
+        <v>3.6</v>
       </c>
       <c r="N53" s="14">
         <f t="shared" si="0"/>
-        <v>13.5</v>
+        <v>12.375</v>
       </c>
       <c r="O53" s="14">
         <f t="shared" si="1"/>
-        <v>1.1076923076923078</v>
+        <v>1.2298136645962734</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="E54" s="1">
-        <v>100</v>
+        <v>164</v>
       </c>
       <c r="F54" s="2">
-        <v>337</v>
+        <v>166</v>
       </c>
       <c r="G54" s="3">
-        <v>2.1</v>
+        <v>0.6</v>
       </c>
       <c r="H54" s="3">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="I54" s="4">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="J54" s="4">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="K54" s="4">
-        <v>7.8</v>
+        <v>1.2</v>
       </c>
       <c r="L54" s="5">
-        <v>15</v>
+        <v>6.5</v>
       </c>
       <c r="N54" s="14">
         <f t="shared" si="0"/>
-        <v>21.0625</v>
+        <v>10.375</v>
       </c>
       <c r="O54" s="14">
         <f t="shared" si="1"/>
-        <v>3.37</v>
+        <v>1.0121951219512195</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>145</v>
+        <v>121</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="E55" s="1">
-        <v>133</v>
+        <v>195</v>
       </c>
       <c r="F55" s="2">
-        <v>410</v>
+        <v>216</v>
       </c>
       <c r="G55" s="3">
-        <v>1.3</v>
+        <v>1.5</v>
       </c>
       <c r="H55" s="3">
         <v>0</v>
       </c>
       <c r="I55" s="4">
-        <v>110</v>
+        <v>32</v>
       </c>
       <c r="J55" s="4">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="K55" s="4">
-        <v>96.7</v>
+        <v>0</v>
       </c>
       <c r="L55" s="5">
-        <v>0.3</v>
+        <v>3</v>
       </c>
       <c r="N55" s="14">
         <f t="shared" si="0"/>
-        <v>25.625</v>
+        <v>13.5</v>
       </c>
       <c r="O55" s="14">
         <f t="shared" si="1"/>
-        <v>3.0827067669172932</v>
+        <v>1.1076923076923078</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="E56" s="1">
-        <v>145</v>
+        <v>100</v>
       </c>
       <c r="F56" s="2">
-        <v>435</v>
+        <v>337</v>
       </c>
       <c r="G56" s="3">
-        <v>0.6</v>
+        <v>2.1</v>
       </c>
       <c r="H56" s="3">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="I56" s="4">
-        <v>117</v>
+        <v>71</v>
       </c>
       <c r="J56" s="4">
-        <v>5.6</v>
+        <v>11</v>
       </c>
       <c r="K56" s="4">
-        <v>83.7</v>
+        <v>7.8</v>
       </c>
       <c r="L56" s="5">
-        <v>4.5</v>
+        <v>15</v>
       </c>
       <c r="N56" s="14">
         <f t="shared" si="0"/>
-        <v>27.1875</v>
+        <v>21.0625</v>
       </c>
       <c r="O56" s="14">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>3.37</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>147</v>
+        <v>123</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>51</v>
+        <v>160</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="E57" s="1">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="F57" s="2">
-        <v>440</v>
+        <v>271</v>
       </c>
       <c r="G57" s="3">
-        <v>1.9</v>
+        <v>1.7</v>
       </c>
       <c r="H57" s="3">
         <v>0</v>
       </c>
       <c r="I57" s="4">
-        <v>114</v>
+        <v>56.2</v>
       </c>
       <c r="J57" s="4">
-        <v>17.8</v>
+        <v>7.6</v>
       </c>
       <c r="K57" s="4">
         <v>0</v>
       </c>
       <c r="L57" s="5">
-        <v>5.6</v>
-      </c>
-      <c r="M57" s="2">
-        <v>21</v>
+        <v>11.9</v>
       </c>
       <c r="N57" s="14">
         <f t="shared" si="0"/>
-        <v>27.5</v>
+        <v>16.9375</v>
       </c>
       <c r="O57" s="14">
         <f t="shared" si="1"/>
-        <v>2.4719101123595504</v>
+        <v>1.456989247311828</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>148</v>
+        <v>124</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>52</v>
+        <v>173</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E58" s="1">
-        <v>160</v>
+        <v>133</v>
       </c>
       <c r="F58" s="2">
-        <v>369</v>
+        <v>410</v>
       </c>
       <c r="G58" s="3">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="H58" s="3">
         <v>0</v>
       </c>
       <c r="I58" s="4">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="J58" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K58" s="4">
-        <v>52</v>
+        <v>96.7</v>
       </c>
       <c r="L58" s="5">
-        <v>4</v>
-      </c>
-      <c r="M58" s="2">
-        <v>20</v>
+        <v>0.3</v>
       </c>
       <c r="N58" s="14">
         <f t="shared" si="0"/>
-        <v>23.0625</v>
+        <v>25.625</v>
       </c>
       <c r="O58" s="14">
         <f t="shared" si="1"/>
-        <v>2.3062499999999999</v>
+        <v>3.0827067669172932</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>149</v>
+        <v>125</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="E59" s="1">
-        <v>53</v>
+        <v>145</v>
       </c>
       <c r="F59" s="2">
-        <v>10</v>
+        <v>435</v>
       </c>
       <c r="G59" s="3">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="H59" s="3">
         <v>0</v>
       </c>
       <c r="I59" s="4">
-        <v>1</v>
+        <v>117</v>
       </c>
       <c r="J59" s="4">
-        <v>1</v>
+        <v>5.6</v>
       </c>
       <c r="K59" s="4">
-        <v>0</v>
+        <v>83.7</v>
       </c>
       <c r="L59" s="5">
-        <v>2</v>
+        <v>4.5</v>
       </c>
       <c r="N59" s="14">
         <f t="shared" si="0"/>
-        <v>0.625</v>
+        <v>27.1875</v>
       </c>
       <c r="O59" s="14">
         <f t="shared" si="1"/>
-        <v>0.18867924528301888</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>150</v>
+        <v>126</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>55</v>
+        <v>172</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="E60" s="1">
-        <v>25</v>
+        <v>178</v>
       </c>
       <c r="F60" s="2">
-        <v>11</v>
+        <v>440</v>
       </c>
       <c r="G60" s="3">
-        <v>0.2</v>
+        <v>1.9</v>
       </c>
       <c r="H60" s="3">
         <v>0</v>
       </c>
       <c r="I60" s="4">
-        <v>2.1</v>
+        <v>114</v>
       </c>
       <c r="J60" s="4">
-        <v>1.8</v>
+        <v>17.8</v>
       </c>
       <c r="K60" s="4">
         <v>0</v>
       </c>
       <c r="L60" s="5">
-        <v>0.8</v>
+        <v>5.6</v>
+      </c>
+      <c r="M60" s="2">
+        <v>21</v>
       </c>
       <c r="N60" s="14">
         <f t="shared" si="0"/>
-        <v>0.6875</v>
+        <v>27.5</v>
       </c>
       <c r="O60" s="14">
         <f t="shared" si="1"/>
-        <v>0.44</v>
+        <v>2.4719101123595504</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61" s="6" t="s">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>56</v>
+        <v>171</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="E61" s="1">
-        <v>9</v>
+        <v>160</v>
       </c>
       <c r="F61" s="2">
-        <v>3.8</v>
+        <v>369</v>
       </c>
       <c r="G61" s="3">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="H61" s="3">
         <v>0</v>
       </c>
       <c r="I61" s="4">
-        <v>0.6</v>
+        <v>84</v>
       </c>
       <c r="J61" s="4">
-        <v>0.2</v>
+        <v>8</v>
       </c>
       <c r="K61" s="4">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="L61" s="5">
-        <v>0.3</v>
+        <v>4</v>
+      </c>
+      <c r="M61" s="2">
+        <v>20</v>
       </c>
       <c r="N61" s="14">
         <f t="shared" si="0"/>
-        <v>0.23749999999999999</v>
+        <v>23.0625</v>
       </c>
       <c r="O61" s="14">
         <f t="shared" si="1"/>
-        <v>0.42222222222222222</v>
+        <v>2.3062499999999999</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B62" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="E62" s="1">
-        <v>13.3</v>
+        <v>53</v>
       </c>
       <c r="F62" s="2">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G62" s="3">
         <v>0</v>
@@ -3895,136 +3970,136 @@
         <v>0</v>
       </c>
       <c r="I62" s="4">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="J62" s="4">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K62" s="4">
         <v>0</v>
       </c>
       <c r="L62" s="5">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="N62" s="14">
         <f t="shared" si="0"/>
-        <v>0.1875</v>
+        <v>0.625</v>
       </c>
       <c r="O62" s="14">
         <f t="shared" si="1"/>
-        <v>0.22556390977443608</v>
+        <v>0.18867924528301888</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A63" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B63" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="E63" s="1">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F63" s="2">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="G63" s="3">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="H63" s="3">
         <v>0</v>
       </c>
       <c r="I63" s="4">
-        <v>8.5</v>
+        <v>2.1</v>
       </c>
       <c r="J63" s="4">
-        <v>4.8</v>
+        <v>1.8</v>
       </c>
       <c r="K63" s="4">
         <v>0</v>
       </c>
       <c r="L63" s="5">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="N63" s="14">
         <f t="shared" si="0"/>
-        <v>2.375</v>
+        <v>0.6875</v>
       </c>
       <c r="O63" s="14">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="E64" s="1">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="F64" s="2">
-        <v>96</v>
+        <v>3.8</v>
       </c>
       <c r="G64" s="3">
-        <v>4.8</v>
+        <v>0.1</v>
       </c>
       <c r="H64" s="3">
-        <v>1.6</v>
+        <v>0</v>
       </c>
       <c r="I64" s="4">
-        <v>16</v>
+        <v>0.6</v>
       </c>
       <c r="J64" s="4">
-        <v>16</v>
+        <v>0.2</v>
       </c>
       <c r="K64" s="4">
         <v>0</v>
       </c>
       <c r="L64" s="5">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="N64" s="14">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>0.23749999999999999</v>
       </c>
       <c r="O64" s="14">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>0.42222222222222222</v>
       </c>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A65" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B65" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="E65" s="1">
-        <v>127</v>
+        <v>13.3</v>
       </c>
       <c r="F65" s="2">
-        <v>127</v>
+        <v>3</v>
       </c>
       <c r="G65" s="3">
         <v>0</v>
@@ -4033,102 +4108,102 @@
         <v>0</v>
       </c>
       <c r="I65" s="4">
-        <v>25.4</v>
+        <v>0.3</v>
       </c>
       <c r="J65" s="4">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="K65" s="4">
         <v>0</v>
       </c>
       <c r="L65" s="5">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="N65" s="14">
         <f t="shared" si="0"/>
-        <v>7.9375</v>
+        <v>0.1875</v>
       </c>
       <c r="O65" s="14">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.22556390977443608</v>
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A66" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B66" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="E66" s="1">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="F66" s="2">
-        <v>90</v>
+        <v>38</v>
       </c>
       <c r="G66" s="3">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="H66" s="3">
         <v>0</v>
       </c>
       <c r="I66" s="4">
-        <v>5.3</v>
+        <v>8.5</v>
       </c>
       <c r="J66" s="4">
-        <v>2.5</v>
+        <v>4.8</v>
       </c>
       <c r="K66" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L66" s="5">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="N66" s="14">
         <f t="shared" si="0"/>
-        <v>5.625</v>
+        <v>2.375</v>
       </c>
       <c r="O66" s="14">
         <f t="shared" si="1"/>
-        <v>3.3333333333333335</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A67" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D67" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B67" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="E67" s="1">
-        <v>135</v>
+        <v>32</v>
       </c>
       <c r="F67" s="2">
-        <v>156</v>
+        <v>96</v>
       </c>
       <c r="G67" s="3">
-        <v>14.2</v>
+        <v>4.8</v>
       </c>
       <c r="H67" s="3">
-        <v>3.6</v>
+        <v>1.6</v>
       </c>
       <c r="I67" s="4">
-        <v>7.1</v>
+        <v>16</v>
       </c>
       <c r="J67" s="4">
-        <v>3.6</v>
+        <v>16</v>
       </c>
       <c r="K67" s="4">
         <v>0</v>
@@ -4137,252 +4212,885 @@
         <v>0</v>
       </c>
       <c r="N67" s="14">
-        <f t="shared" ref="N67:N72" si="2">F67*15/240</f>
-        <v>9.75</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="O67" s="14">
-        <f t="shared" ref="O67" si="3">F67/E67</f>
-        <v>1.1555555555555554</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A68" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D68" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="E68" s="1">
+        <v>127</v>
+      </c>
+      <c r="F68" s="2">
+        <v>127</v>
+      </c>
+      <c r="G68" s="3">
+        <v>0</v>
+      </c>
+      <c r="H68" s="3">
+        <v>0</v>
+      </c>
+      <c r="I68" s="4">
+        <v>25.4</v>
+      </c>
+      <c r="J68" s="4">
+        <v>0</v>
+      </c>
+      <c r="K68" s="4">
+        <v>0</v>
+      </c>
+      <c r="L68" s="5">
+        <v>0</v>
+      </c>
+      <c r="N68" s="14">
+        <f t="shared" si="0"/>
+        <v>7.9375</v>
+      </c>
+      <c r="O68" s="14">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A69" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E69" s="1">
+        <v>27</v>
+      </c>
+      <c r="F69" s="2">
+        <v>90</v>
+      </c>
+      <c r="G69" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H69" s="3">
+        <v>0</v>
+      </c>
+      <c r="I69" s="4">
+        <v>5.3</v>
+      </c>
+      <c r="J69" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="K69" s="4">
+        <v>3</v>
+      </c>
+      <c r="L69" s="5">
+        <v>1.2</v>
+      </c>
+      <c r="N69" s="14">
+        <f t="shared" si="0"/>
+        <v>5.625</v>
+      </c>
+      <c r="O69" s="14">
+        <f t="shared" si="1"/>
+        <v>3.3333333333333335</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A70" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E70" s="1">
+        <v>135</v>
+      </c>
+      <c r="F70" s="2">
+        <v>156</v>
+      </c>
+      <c r="G70" s="3">
+        <v>14.2</v>
+      </c>
+      <c r="H70" s="3">
+        <v>3.6</v>
+      </c>
+      <c r="I70" s="4">
+        <v>7.1</v>
+      </c>
+      <c r="J70" s="4">
+        <v>3.6</v>
+      </c>
+      <c r="K70" s="4">
+        <v>0</v>
+      </c>
+      <c r="L70" s="5">
+        <v>0</v>
+      </c>
+      <c r="N70" s="14">
+        <f t="shared" ref="N70:N75" si="2">F70*15/240</f>
+        <v>9.75</v>
+      </c>
+      <c r="O70" s="14">
+        <f t="shared" ref="O70" si="3">F70/E70</f>
+        <v>1.1555555555555554</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A71" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E71" s="1">
         <v>93.5</v>
       </c>
-      <c r="F68" s="2">
+      <c r="F71" s="2">
         <v>17</v>
       </c>
-      <c r="G68" s="3">
+      <c r="G71" s="3">
         <v>0.2</v>
       </c>
-      <c r="H68" s="3">
-        <v>0</v>
-      </c>
-      <c r="I68" s="4">
+      <c r="H71" s="3">
+        <v>0</v>
+      </c>
+      <c r="I71" s="4">
         <v>4</v>
       </c>
-      <c r="J68" s="4">
+      <c r="J71" s="4">
         <v>1.1000000000000001</v>
       </c>
-      <c r="K68" s="4">
+      <c r="K71" s="4">
         <v>3.5</v>
       </c>
-      <c r="L68" s="5">
+      <c r="L71" s="5">
         <v>0.6</v>
       </c>
-      <c r="N68" s="14">
+      <c r="N71" s="14">
         <f t="shared" si="2"/>
         <v>1.0625</v>
       </c>
-      <c r="O68" s="14">
-        <f>F68/E68</f>
+      <c r="O71" s="14">
+        <f>F71/E71</f>
         <v>0.18181818181818182</v>
-      </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A69" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E69" s="1">
-        <v>312</v>
-      </c>
-      <c r="F69" s="2">
-        <v>290</v>
-      </c>
-      <c r="G69" s="3">
-        <v>2.9</v>
-      </c>
-      <c r="H69" s="3">
-        <v>0</v>
-      </c>
-      <c r="I69" s="4">
-        <v>60</v>
-      </c>
-      <c r="J69" s="4">
-        <v>6.7</v>
-      </c>
-      <c r="K69" s="4">
-        <v>47</v>
-      </c>
-      <c r="L69" s="5">
-        <v>6</v>
-      </c>
-      <c r="N69" s="14">
-        <f t="shared" si="2"/>
-        <v>18.125</v>
-      </c>
-      <c r="O69" s="14">
-        <f t="shared" ref="O69:O72" si="4">F69/E69</f>
-        <v>0.92948717948717952</v>
-      </c>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A70" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E70" s="1">
-        <v>0</v>
-      </c>
-      <c r="F70" s="2">
-        <v>0</v>
-      </c>
-      <c r="G70" s="3">
-        <v>0</v>
-      </c>
-      <c r="H70" s="3">
-        <v>0</v>
-      </c>
-      <c r="I70" s="4">
-        <v>0</v>
-      </c>
-      <c r="J70" s="4">
-        <v>0</v>
-      </c>
-      <c r="K70" s="4">
-        <v>0</v>
-      </c>
-      <c r="L70" s="5">
-        <v>0</v>
-      </c>
-      <c r="N70" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O70" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A71" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E71" s="1">
-        <v>238</v>
-      </c>
-      <c r="F71" s="2">
-        <v>38</v>
-      </c>
-      <c r="G71" s="3">
-        <v>0</v>
-      </c>
-      <c r="H71" s="3">
-        <v>0</v>
-      </c>
-      <c r="I71" s="4">
-        <v>14.2</v>
-      </c>
-      <c r="J71" s="4">
-        <v>0</v>
-      </c>
-      <c r="K71" s="4">
-        <v>4.8</v>
-      </c>
-      <c r="L71" s="5">
-        <v>0</v>
-      </c>
-      <c r="N71" s="14">
-        <f t="shared" si="2"/>
-        <v>2.375</v>
-      </c>
-      <c r="O71" s="14">
-        <f t="shared" si="4"/>
-        <v>0.15966386554621848</v>
       </c>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A72" s="6" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>91</v>
+        <v>150</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="E72" s="1">
-        <v>256</v>
+        <v>142</v>
       </c>
       <c r="F72" s="2">
-        <v>224</v>
+        <v>27</v>
       </c>
       <c r="G72" s="3">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="H72" s="3">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="I72" s="4">
-        <v>43.2</v>
+        <v>6.1</v>
       </c>
       <c r="J72" s="4">
-        <v>0</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="K72" s="4">
-        <v>38.4</v>
+        <v>2.5</v>
       </c>
       <c r="L72" s="5">
-        <v>1.6</v>
+        <v>1.3</v>
       </c>
       <c r="N72" s="14">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>1.6875</v>
       </c>
       <c r="O72" s="14">
-        <f t="shared" si="4"/>
-        <v>0.875</v>
+        <f>F72/E72</f>
+        <v>0.19014084507042253</v>
       </c>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A73" s="6" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="B73" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E73" s="1">
+        <v>168</v>
+      </c>
+      <c r="F73" s="2">
+        <v>90</v>
+      </c>
+      <c r="G73" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H73" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="I73" s="4">
+        <v>20</v>
+      </c>
+      <c r="J73" s="4">
+        <v>9.6</v>
+      </c>
+      <c r="K73" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="L73" s="5">
+        <v>4.8</v>
+      </c>
+      <c r="N73" s="14">
+        <f t="shared" si="2"/>
+        <v>5.625</v>
+      </c>
+      <c r="O73" s="14">
+        <f>F73/E73</f>
+        <v>0.5357142857142857</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A74" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E74" s="1">
+        <v>206</v>
+      </c>
+      <c r="F74" s="2">
+        <v>70</v>
+      </c>
+      <c r="G74" s="3">
+        <v>1</v>
+      </c>
+      <c r="H74" s="3">
+        <v>0</v>
+      </c>
+      <c r="I74" s="4">
+        <v>14</v>
+      </c>
+      <c r="J74" s="4">
+        <v>3.9</v>
+      </c>
+      <c r="K74" s="4">
+        <v>8</v>
+      </c>
+      <c r="L74" s="5">
+        <v>2</v>
+      </c>
+      <c r="N74" s="14">
+        <f t="shared" si="2"/>
+        <v>4.375</v>
+      </c>
+      <c r="O74" s="14">
+        <f>F74/E74</f>
+        <v>0.33980582524271846</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A75" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E75" s="1">
+        <v>1423</v>
+      </c>
+      <c r="F75" s="2">
+        <v>19</v>
+      </c>
+      <c r="G75" s="3">
+        <v>0</v>
+      </c>
+      <c r="H75" s="3">
+        <v>0</v>
+      </c>
+      <c r="I75" s="4">
+        <v>9.5</v>
+      </c>
+      <c r="J75" s="4">
+        <v>0</v>
+      </c>
+      <c r="K75" s="4">
+        <v>0</v>
+      </c>
+      <c r="L75" s="5">
+        <v>0</v>
+      </c>
+      <c r="N75" s="14">
+        <f t="shared" si="2"/>
+        <v>1.1875</v>
+      </c>
+      <c r="O75" s="14">
+        <f>F75/E75</f>
+        <v>1.3352073085031623E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A76" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E76" s="1">
+        <v>312</v>
+      </c>
+      <c r="F76" s="2">
+        <v>290</v>
+      </c>
+      <c r="G76" s="3">
+        <v>2.9</v>
+      </c>
+      <c r="H76" s="3">
+        <v>0</v>
+      </c>
+      <c r="I76" s="4">
+        <v>60</v>
+      </c>
+      <c r="J76" s="4">
+        <v>6.7</v>
+      </c>
+      <c r="K76" s="4">
+        <v>47</v>
+      </c>
+      <c r="L76" s="5">
+        <v>6</v>
+      </c>
+      <c r="N76" s="14">
+        <f t="shared" ref="N76:N86" si="4">F76*15/240</f>
+        <v>18.125</v>
+      </c>
+      <c r="O76" s="14">
+        <f t="shared" ref="O76:O81" si="5">F76/E76</f>
+        <v>0.92948717948717952</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A77" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E77" s="1">
+        <v>0</v>
+      </c>
+      <c r="F77" s="2">
+        <v>0</v>
+      </c>
+      <c r="G77" s="3">
+        <v>0</v>
+      </c>
+      <c r="H77" s="3">
+        <v>0</v>
+      </c>
+      <c r="I77" s="4">
+        <v>0</v>
+      </c>
+      <c r="J77" s="4">
+        <v>0</v>
+      </c>
+      <c r="K77" s="4">
+        <v>0</v>
+      </c>
+      <c r="L77" s="5">
+        <v>0</v>
+      </c>
+      <c r="N77" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O77" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A78" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E78" s="1">
+        <v>238</v>
+      </c>
+      <c r="F78" s="2">
+        <v>38</v>
+      </c>
+      <c r="G78" s="3">
+        <v>0</v>
+      </c>
+      <c r="H78" s="3">
+        <v>0</v>
+      </c>
+      <c r="I78" s="4">
+        <v>14.2</v>
+      </c>
+      <c r="J78" s="4">
+        <v>0</v>
+      </c>
+      <c r="K78" s="4">
+        <v>4.8</v>
+      </c>
+      <c r="L78" s="5">
+        <v>0</v>
+      </c>
+      <c r="N78" s="14">
+        <f t="shared" si="4"/>
+        <v>2.375</v>
+      </c>
+      <c r="O78" s="14">
+        <f t="shared" si="5"/>
+        <v>0.15966386554621848</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A79" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E79" s="1">
+        <v>256</v>
+      </c>
+      <c r="F79" s="2">
+        <v>224</v>
+      </c>
+      <c r="G79" s="3">
+        <v>0</v>
+      </c>
+      <c r="H79" s="3">
+        <v>0</v>
+      </c>
+      <c r="I79" s="4">
+        <v>43.2</v>
+      </c>
+      <c r="J79" s="4">
+        <v>0</v>
+      </c>
+      <c r="K79" s="4">
+        <v>38.4</v>
+      </c>
+      <c r="L79" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="N79" s="14">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="O79" s="14">
+        <f t="shared" si="5"/>
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A80" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E80" s="1">
+        <v>224</v>
+      </c>
+      <c r="F80" s="2">
+        <v>480</v>
+      </c>
+      <c r="G80" s="3">
+        <v>36</v>
+      </c>
+      <c r="H80" s="3">
+        <v>4</v>
+      </c>
+      <c r="I80" s="4">
+        <v>32</v>
+      </c>
+      <c r="J80" s="4">
+        <v>8</v>
+      </c>
+      <c r="K80" s="4">
+        <v>8</v>
+      </c>
+      <c r="L80" s="5">
+        <v>16</v>
+      </c>
+      <c r="N80" s="14">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="O80" s="14">
+        <f t="shared" si="5"/>
+        <v>2.1428571428571428</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A81" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E81" s="1">
+        <v>249.3</v>
+      </c>
+      <c r="F81" s="2">
+        <v>1122</v>
+      </c>
+      <c r="G81" s="3">
+        <v>125</v>
+      </c>
+      <c r="H81" s="3">
+        <v>22.8</v>
+      </c>
+      <c r="I81" s="4">
+        <v>6.2</v>
+      </c>
+      <c r="J81" s="4">
+        <v>0</v>
+      </c>
+      <c r="K81" s="4">
+        <v>6.2</v>
+      </c>
+      <c r="L81" s="5">
+        <v>0</v>
+      </c>
+      <c r="N81" s="14">
+        <f t="shared" si="4"/>
+        <v>70.125</v>
+      </c>
+      <c r="O81" s="14">
+        <f t="shared" si="5"/>
+        <v>4.5006016847172079</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A82" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C82" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="C73" s="1" t="s">
-        <v>64</v>
+      <c r="D82" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E82" s="1">
+        <v>232</v>
+      </c>
+      <c r="F82" s="2">
+        <v>280</v>
+      </c>
+      <c r="G82" s="3">
+        <v>24</v>
+      </c>
+      <c r="H82" s="3">
+        <v>0</v>
+      </c>
+      <c r="I82" s="4">
+        <v>16</v>
+      </c>
+      <c r="J82" s="4">
+        <v>0</v>
+      </c>
+      <c r="K82" s="4">
+        <v>0</v>
+      </c>
+      <c r="L82" s="5">
+        <v>4</v>
+      </c>
+      <c r="N82" s="14">
+        <f t="shared" si="4"/>
+        <v>17.5</v>
+      </c>
+      <c r="O82" s="14">
+        <f t="shared" ref="O82:O86" si="6">F82/E82</f>
+        <v>1.2068965517241379</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A83" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E83" s="1">
+        <v>240</v>
+      </c>
+      <c r="F83" s="2">
+        <v>1032</v>
+      </c>
+      <c r="G83" s="3">
+        <v>104</v>
+      </c>
+      <c r="H83" s="3">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="I83" s="4">
+        <v>14.4</v>
+      </c>
+      <c r="J83" s="4">
+        <v>0</v>
+      </c>
+      <c r="K83" s="4">
+        <v>11.2</v>
+      </c>
+      <c r="L83" s="5">
+        <v>3.2</v>
+      </c>
+      <c r="N83" s="14">
+        <f t="shared" si="4"/>
+        <v>64.5</v>
+      </c>
+      <c r="O83" s="14">
+        <f t="shared" si="6"/>
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A84" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E84" s="1">
+        <v>250</v>
+      </c>
+      <c r="F84" s="2">
+        <v>948</v>
+      </c>
+      <c r="G84" s="3">
+        <v>91.5</v>
+      </c>
+      <c r="H84" s="3">
+        <v>12.5</v>
+      </c>
+      <c r="I84" s="4">
+        <v>36.6</v>
+      </c>
+      <c r="J84" s="4">
+        <v>1.7</v>
+      </c>
+      <c r="K84" s="4">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="L84" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="N84" s="14">
+        <f t="shared" si="4"/>
+        <v>59.25</v>
+      </c>
+      <c r="O84" s="14">
+        <f t="shared" si="6"/>
+        <v>3.7919999999999998</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A85" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E85" s="1">
+        <v>224</v>
+      </c>
+      <c r="F85" s="2">
+        <v>320</v>
+      </c>
+      <c r="G85" s="3">
+        <v>32</v>
+      </c>
+      <c r="H85" s="3">
+        <v>4</v>
+      </c>
+      <c r="I85" s="4">
+        <v>32</v>
+      </c>
+      <c r="J85" s="4">
+        <v>0</v>
+      </c>
+      <c r="K85" s="4">
+        <v>24</v>
+      </c>
+      <c r="L85" s="5">
+        <v>0</v>
+      </c>
+      <c r="N85" s="14">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="O85" s="14">
+        <f t="shared" si="6"/>
+        <v>1.4285714285714286</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A86" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E86" s="1">
+        <v>227</v>
+      </c>
+      <c r="F86" s="2">
+        <v>440</v>
+      </c>
+      <c r="G86" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="H86" s="3">
+        <v>0</v>
+      </c>
+      <c r="I86" s="4">
+        <v>112</v>
+      </c>
+      <c r="J86" s="4">
+        <v>3.1</v>
+      </c>
+      <c r="K86" s="4">
+        <v>88</v>
+      </c>
+      <c r="L86" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="N86" s="14">
+        <f t="shared" si="4"/>
+        <v>27.5</v>
+      </c>
+      <c r="O86" s="14">
+        <f t="shared" si="6"/>
+        <v>1.9383259911894273</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: dup entry salad
</commit_message>
<xml_diff>
--- a/Salad/Salad_planner_database.xlsx
+++ b/Salad/Salad_planner_database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yolandatiao/Documents/YoloCookBlob/Salad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2932029-2172-354E-B4F2-069FE6161085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B17BD5D-077D-B74A-83BA-5DA4101B2E5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15700" xr2:uid="{01A3236E-6E79-A74A-AA94-09FBDF0EA52A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="197">
   <si>
     <t>Name</t>
   </si>
@@ -624,6 +624,9 @@
   </si>
   <si>
     <t>Cranberry Sauce</t>
+  </si>
+  <si>
+    <t>HDS_6</t>
   </si>
 </sst>
 </file>
@@ -1076,8 +1079,8 @@
   <dimension ref="A1:O86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B57" sqref="B57"/>
+      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C83" sqref="C83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4868,7 +4871,7 @@
         <v>53</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>141</v>
+        <v>164</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>163</v>
@@ -4914,7 +4917,7 @@
         <v>53</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>164</v>
+        <v>191</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>165</v>
@@ -4960,7 +4963,7 @@
         <v>53</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>189</v>
@@ -5006,7 +5009,7 @@
         <v>53</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>190</v>
@@ -5052,7 +5055,7 @@
         <v>53</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>195</v>

</xml_diff>